<commit_message>
clean up global settings
</commit_message>
<xml_diff>
--- a/case/testcase.xlsx
+++ b/case/testcase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98C6B5AB-ED49-4273-9D9A-091C9611CC9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{22E4E051-061E-433E-815B-EAFCEF0B2F30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
handle exception of empty json expression
</commit_message>
<xml_diff>
--- a/case/testcase.xlsx
+++ b/case/testcase.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{22E4E051-061E-433E-815B-EAFCEF0B2F30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5776D2-5CC4-464D-AF27-FDC78B5C9214}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
     <sheet name="GitHub" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>CaseId</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://github.com/login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -110,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>data1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>数据依赖字段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,10 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://github.com/session</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>html:input type="hidden" name="authenticity_token" .*value="(.*?)":1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -137,10 +125,6 @@
     <t>github-003</t>
   </si>
   <si>
-    <t>https://github.com/discover</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>discover_repositories</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,10 +152,18 @@
     <t>github-004</t>
   </si>
   <si>
+    <t>将discover repository返回的一个项目置星</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Site Specific</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>GitHub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Action Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -181,6 +173,14 @@
   </si>
   <si>
     <t>URL后缀依赖的返回数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>html:input type="hidden" name="authenticity_token" .*value="(.*?)":6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>html:&lt;a itemprop="name codeRepository".*href="(.*?)"&gt;:0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -208,6 +208,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>test_star_a_project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>test_get_login_page</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -216,14 +220,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>test_login_failure_no_token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试未提供authenticity_token情况下，登录失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>github-login-001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>github-login-003</t>
+  </si>
+  <si>
     <t>github-login-004</t>
   </si>
   <si>
@@ -262,11 +281,32 @@
     <t>github-login-005</t>
   </si>
   <si>
+    <t>Your browser did something unexpected. Please contact us if the problem persists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Forgot password?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>You can’t perform that action at this time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>/discover</t>
+  </si>
+  <si>
+    <t>/session</t>
+  </si>
+  <si>
+    <t>期望返回Json内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -627,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -651,12 +691,12 @@
     <col min="18" max="18" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -665,25 +705,25 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
         <v>2</v>
@@ -704,203 +744,276 @@
         <v>8</v>
       </c>
       <c r="R1" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" t="s">
         <v>9</v>
       </c>
       <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
         <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>12</v>
       </c>
       <c r="P2" s="6">
         <v>200</v>
       </c>
       <c r="Q2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P3" s="6">
         <v>200</v>
       </c>
       <c r="Q3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="R3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="P4" s="6">
-        <v>200</v>
+        <v>422</v>
       </c>
       <c r="Q4" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="R4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>62</v>
       </c>
       <c r="P5" s="6">
         <v>200</v>
       </c>
       <c r="Q5" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="R5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="4"/>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="P6" s="6">
         <v>200</v>
       </c>
       <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="6">
+        <v>200</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="R6" t="s">
-        <v>52</v>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{9A11CE41-2C84-42B4-8F5F-A00257C4E33D}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{9A60F31F-51B4-42EF-8CF9-28288701879D}"/>
-    <hyperlink ref="J6" r:id="rId3" xr:uid="{C7A696B7-2F0C-4D3D-8F2C-2DAC4A92D1A1}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{DEF39FB4-D64F-4A03-99B3-5616543A049C}"/>
-    <hyperlink ref="J3" r:id="rId5" xr:uid="{9FBC9E1F-DE06-4B96-A8BA-82018B21356D}"/>
+    <hyperlink ref="J5" r:id="rId1" display="https://github.com/session" xr:uid="{9A11CE41-2C84-42B4-8F5F-A00257C4E33D}"/>
+    <hyperlink ref="J2" r:id="rId2" display="https://github.com/login" xr:uid="{9A60F31F-51B4-42EF-8CF9-28288701879D}"/>
+    <hyperlink ref="J7" r:id="rId3" display="https://github.com/discover" xr:uid="{C7A696B7-2F0C-4D3D-8F2C-2DAC4A92D1A1}"/>
+    <hyperlink ref="J8" r:id="rId4" display="https://github.com/discover" xr:uid="{584F4C9B-5C9F-4E76-BEE0-3D5D505A89AC}"/>
+    <hyperlink ref="J6" r:id="rId5" display="https://github.com/session" xr:uid="{DEF39FB4-D64F-4A03-99B3-5616543A049C}"/>
+    <hyperlink ref="J3" r:id="rId6" display="https://github.com/discover" xr:uid="{9FBC9E1F-DE06-4B96-A8BA-82018B21356D}"/>
+    <hyperlink ref="J4" r:id="rId7" display="https://github.com/session" xr:uid="{DEF6A5D9-D66A-4763-83BA-06EA23AA433D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -923,15 +1036,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>